<commit_message>
visualised feature importance for all models
</commit_message>
<xml_diff>
--- a/conversion_rate/Models_Scores.xlsx
+++ b/conversion_rate/Models_Scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\Jedha\Fullstack\Projects\Bloc_3\conversion_rate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9C01E0-EE30-46C8-A3B7-DAFAB431A31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C662943-2AD8-47C7-B885-B02242734C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9820" yWindow="2070" windowWidth="15860" windowHeight="11160" xr2:uid="{2E13571D-FE81-43C3-9B41-70477AFD86FF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2E13571D-FE81-43C3-9B41-70477AFD86FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -43,28 +43,28 @@
     <t>Model</t>
   </si>
   <si>
-    <t>F1 score on train (test)</t>
-  </si>
-  <si>
-    <t>F1 score on train (train)</t>
-  </si>
-  <si>
-    <t>F1 score on test</t>
-  </si>
-  <si>
-    <t>Adaboost Tree with GridSearch - iteration 1</t>
-  </si>
-  <si>
-    <t>Adaboost Tree with GridSearch - iteration 2</t>
-  </si>
-  <si>
-    <t>Xgboost - iteration 3</t>
-  </si>
-  <si>
-    <t>Voting LogReg, Adaboost tree,Xgboost</t>
-  </si>
-  <si>
-    <t>Logistic Regression - Multivariate</t>
+    <t>Adaboost_w_Decision_Trees</t>
+  </si>
+  <si>
+    <t>Xgboost</t>
+  </si>
+  <si>
+    <t>Voting_LogReg_Adaboost_w_DT1_Xgboost</t>
+  </si>
+  <si>
+    <t>LogReg_Multivariate</t>
+  </si>
+  <si>
+    <t>F1_score_on_train_labelled</t>
+  </si>
+  <si>
+    <t>F1_score_on_test_labelled</t>
+  </si>
+  <si>
+    <t>F1_score_on_test_unlabelled</t>
+  </si>
+  <si>
+    <t>Training_time_seconds</t>
   </si>
 </sst>
 </file>
@@ -113,7 +113,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -212,14 +226,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{341C7027-46D4-434E-B264-F227291C2E46}" name="Tableau1" displayName="Tableau1" ref="A1:E6" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E6" xr:uid="{341C7027-46D4-434E-B264-F227291C2E46}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F6FCC2C2-3AE9-4535-82D6-394242F4C2E0}" name="Sumbission number" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{B06DF2F4-30D8-4676-BC14-30ACECB723F8}" name="Model" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{F8775B3F-4109-47C5-873E-8863BC1FD45B}" name="F1 score on train (train)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{D2E970C9-5903-43CB-A7E7-BD600B78733D}" name="F1 score on train (test)" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{32AD53B5-D21D-4389-AEF2-F9CB27524B7A}" name="F1 score on test" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{341C7027-46D4-434E-B264-F227291C2E46}" name="Tableau1" displayName="Tableau1" ref="A1:F5" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A1:F5" xr:uid="{341C7027-46D4-434E-B264-F227291C2E46}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{F6FCC2C2-3AE9-4535-82D6-394242F4C2E0}" name="Sumbission number" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B06DF2F4-30D8-4676-BC14-30ACECB723F8}" name="Model" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F8775B3F-4109-47C5-873E-8863BC1FD45B}" name="F1_score_on_train_labelled" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D2E970C9-5903-43CB-A7E7-BD600B78733D}" name="F1_score_on_test_labelled" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{32AD53B5-D21D-4389-AEF2-F9CB27524B7A}" name="F1_score_on_test_unlabelled" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{9FC25B2E-0177-4AAC-AB3A-5045E3B8F13D}" name="Training_time_seconds" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -522,22 +537,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6408BD8-C62A-48D1-B2C9-508E5BDE8862}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.7265625" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" customWidth="1"/>
+    <col min="4" max="4" width="29.90625" customWidth="1"/>
+    <col min="5" max="5" width="27.1796875" customWidth="1"/>
+    <col min="6" max="6" width="21.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,21 +561,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>0.76545070847150998</v>
@@ -570,73 +589,68 @@
       <c r="E2" s="1">
         <v>0.75461500000000004</v>
       </c>
+      <c r="F2" s="1">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.764460696</v>
+        <v>0.76986754966887405</v>
       </c>
       <c r="D3" s="1">
-        <v>0.75670945157500002</v>
+        <v>0.74481514878268695</v>
       </c>
       <c r="E3" s="1">
-        <v>0.74106700000000003</v>
+        <v>0.75526700000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.76986754966887405</v>
+        <v>0.77084112149532702</v>
       </c>
       <c r="D4" s="1">
-        <v>0.74481514878268695</v>
+        <v>0.74895397489539695</v>
       </c>
       <c r="E4" s="1">
-        <v>0.75526700000000002</v>
+        <v>0.75858400000000004</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>0.77084112149532702</v>
+        <v>0.76851364559055702</v>
       </c>
       <c r="D5" s="1">
-        <v>0.74895397489539695</v>
+        <v>0.74849578820697904</v>
       </c>
       <c r="E5" s="1">
-        <v>0.75858400000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.76851364559055702</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.74849578820697904</v>
-      </c>
-      <c r="E6" s="1">
         <v>0.75862099999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>22.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added comments, minor edits
</commit_message>
<xml_diff>
--- a/conversion_rate/Models_Scores.xlsx
+++ b/conversion_rate/Models_Scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\Jedha\Fullstack\Projects\Bloc_3\conversion_rate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C662943-2AD8-47C7-B885-B02242734C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC7D6ED-BBFF-4079-804E-BD3398867C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2E13571D-FE81-43C3-9B41-70477AFD86FF}"/>
+    <workbookView xWindow="-28920" yWindow="2790" windowWidth="29040" windowHeight="17520" xr2:uid="{2E13571D-FE81-43C3-9B41-70477AFD86FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>Xgboost</t>
   </si>
   <si>
-    <t>Voting_LogReg_Adaboost_w_DT1_Xgboost</t>
-  </si>
-  <si>
     <t>LogReg_Multivariate</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>Training_time_seconds</t>
+  </si>
+  <si>
+    <t>Voting_LogReg_Adaboost_w_DT_Xgboost</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -561,16 +561,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>0.76545070847150998</v>
@@ -638,7 +638,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>0.76851364559055702</v>

</xml_diff>